<commit_message>
Time Record - Evening - 14 May 2025
</commit_message>
<xml_diff>
--- a/TestData/LV_TMTT0013748_VerifyNewTitleRateSheetAvailability_CalculatedAmountOnTimeRecordManagerAfterAddingRateSheet.xlsx
+++ b/TestData/LV_TMTT0013748_VerifyNewTitleRateSheetAvailability_CalculatedAmountOnTimeRecordManagerAfterAddingRateSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83ACB5CA-395E-4D0A-B822-FDFBC7323962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97536602-1EC4-4A7A-8616-37F4AE2C5CEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="763" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="763" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="8" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="111">
   <si>
     <t>Rate Sheet</t>
   </si>
@@ -261,33 +261,15 @@
     <t>Financial Analyst Rate</t>
   </si>
   <si>
-    <t>Brad Kay</t>
-  </si>
-  <si>
-    <t>Brett Ryan</t>
-  </si>
-  <si>
     <t>5</t>
   </si>
   <si>
     <t>Drew Koecher</t>
   </si>
   <si>
-    <t>Alexander Drews</t>
-  </si>
-  <si>
     <t>Coartney Trone</t>
   </si>
   <si>
-    <t>Roman Debald</t>
-  </si>
-  <si>
-    <t>Bryan Loh</t>
-  </si>
-  <si>
-    <t>Jack Berka</t>
-  </si>
-  <si>
     <t>StdUser</t>
   </si>
   <si>
@@ -369,31 +351,31 @@
     <t>UpdatedHours</t>
   </si>
   <si>
-    <t>Hagen Machhold</t>
-  </si>
-  <si>
     <t>Liz Hedgcock</t>
   </si>
   <si>
     <t>Michael Graham</t>
   </si>
   <si>
-    <t>William Peluchiwski</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Need to add on TT Beta Grp </t>
-  </si>
-  <si>
-    <t>Qi Chen</t>
-  </si>
-  <si>
-    <t>Garrett Riffe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ayati Arvind </t>
-  </si>
-  <si>
     <t>BUS - Business Services</t>
+  </si>
+  <si>
+    <t>Bryce Schilling</t>
+  </si>
+  <si>
+    <t>Raj Desai</t>
+  </si>
+  <si>
+    <t>Gordon Bolton</t>
+  </si>
+  <si>
+    <t>Blake Dickey</t>
+  </si>
+  <si>
+    <t>Bryan Walker</t>
+  </si>
+  <si>
+    <t>Joseph W. Swanson</t>
   </si>
 </sst>
 </file>
@@ -1264,24 +1246,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1301,12 +1283,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1329,22 +1311,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1356,7 +1338,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{351367AD-7436-4842-8EB6-D7DC6164D492}">
   <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -1473,7 +1455,7 @@
         <v>30</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AD1" s="1" t="s">
         <v>31</v>
@@ -1493,7 +1475,7 @@
         <v>60</v>
       </c>
       <c r="D2" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="E2" t="s">
         <v>34</v>
@@ -1526,13 +1508,13 @@
         <v>2</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="R2" t="s">
         <v>40</v>
@@ -1541,7 +1523,7 @@
         <v>40</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="U2" t="s">
         <v>41</v>
@@ -1562,13 +1544,13 @@
         <v>45</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="AC2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="AD2" t="s">
         <v>46</v>
@@ -1596,24 +1578,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1674,7 +1656,7 @@
         <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D2" t="s">
         <v>57</v>
@@ -1717,101 +1699,101 @@
         <v>62</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1824,8 +1806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1854,24 +1836,19 @@
         <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C2" t="s">
         <v>64</v>
       </c>
-      <c r="D2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>80</v>
-      </c>
+      <c r="E2" s="14"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>66</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C3" t="s">
         <v>64</v>
@@ -1882,7 +1859,7 @@
         <v>67</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
       <c r="C4" t="s">
         <v>64</v>
@@ -1893,21 +1870,19 @@
         <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C5" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="14" t="s">
-        <v>72</v>
-      </c>
+      <c r="E5" s="14"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>69</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>73</v>
+        <v>105</v>
       </c>
       <c r="C6" t="s">
         <v>64</v>
@@ -1918,28 +1893,24 @@
         <v>70</v>
       </c>
       <c r="B7" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C7" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="14" t="s">
-        <v>76</v>
-      </c>
+      <c r="E7" s="14"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>71</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C8" t="s">
         <v>64</v>
       </c>
-      <c r="E8" s="14" t="s">
-        <v>115</v>
-      </c>
+      <c r="E8" s="14"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -1951,9 +1922,7 @@
       <c r="C9" t="s">
         <v>64</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>79</v>
-      </c>
+      <c r="D9" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Time Record Manager - 8th July 2025
</commit_message>
<xml_diff>
--- a/TestData/LV_TMTT0013748_VerifyNewTitleRateSheetAvailability_CalculatedAmountOnTimeRecordManagerAfterAddingRateSheet.xlsx
+++ b/TestData/LV_TMTT0013748_VerifyNewTitleRateSheetAvailability_CalculatedAmountOnTimeRecordManagerAfterAddingRateSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2659FC0-2F83-4944-8795-BC36346DDD16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C4E970C-B1EA-44B2-A9D1-D731B642E32C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="763" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="763" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="8" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="110">
   <si>
     <t>Rate Sheet</t>
   </si>
@@ -223,9 +223,6 @@
   </si>
   <si>
     <t>Sonika Goyal</t>
-  </si>
-  <si>
-    <t>Board Advisory Services (BAS)</t>
   </si>
   <si>
     <t>FVA</t>
@@ -1233,7 +1230,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -1246,24 +1243,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" t="s">
         <v>76</v>
-      </c>
-      <c r="B2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C2" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1283,12 +1280,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1311,22 +1308,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1338,8 +1335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{351367AD-7436-4842-8EB6-D7DC6164D492}">
   <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1455,7 +1452,7 @@
         <v>30</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AD1" s="1" t="s">
         <v>31</v>
@@ -1472,10 +1469,10 @@
         <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E2" t="s">
         <v>34</v>
@@ -1508,13 +1505,13 @@
         <v>2</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="R2" t="s">
         <v>40</v>
@@ -1523,7 +1520,7 @@
         <v>40</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="U2" t="s">
         <v>41</v>
@@ -1538,19 +1535,19 @@
         <v>44</v>
       </c>
       <c r="Y2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Z2" t="s">
         <v>45</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AB2" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AC2" t="s">
         <v>90</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>91</v>
       </c>
       <c r="AD2" t="s">
         <v>46</v>
@@ -1578,24 +1575,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1656,7 +1653,7 @@
         <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>57</v>
@@ -1696,104 +1693,104 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="D1" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>98</v>
-      </c>
       <c r="C6" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1825,7 +1822,7 @@
         <v>49</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -1833,82 +1830,82 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E2" s="14"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E5" s="14"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E7" s="14"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E8" s="14"/>
     </row>
@@ -1917,10 +1914,10 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D9" s="5"/>
     </row>

</xml_diff>